<commit_message>
Added all board files and things
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Viehmann_GPS_2015_BOM" localSheetId="0">Sheet1!$A$1:$I$11</definedName>
+    <definedName name="Viehmann_GPS_2015_BOM" localSheetId="0">Sheet1!$A$1:$G$11</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Qty</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PROD_ID</t>
-  </si>
-  <si>
-    <t>VALUE</t>
-  </si>
-  <si>
     <t>GPS_FGPMMOPA6H</t>
   </si>
   <si>
@@ -158,15 +152,9 @@
     <t>Battery Holders</t>
   </si>
   <si>
-    <t>BATT-08044</t>
-  </si>
-  <si>
     <t>LD1117#50</t>
   </si>
   <si>
-    <t>V_REG_MIC2920</t>
-  </si>
-  <si>
     <t>SOT223</t>
   </si>
   <si>
@@ -185,17 +173,63 @@
     <t>SMD antenna connector- WRL-09144</t>
   </si>
   <si>
-    <t>CONN-09193</t>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>http://www.adafruit.com/products/790</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=182459838&amp;uq=635818978589928070</t>
+  </si>
+  <si>
+    <t>V_REG_LD1117</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/U.FL-R-SMT(01)/H9161-ND/513010</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/10592</t>
+  </si>
+  <si>
+    <t>1206 LED</t>
+  </si>
+  <si>
+    <t>Standard Screw Terminals</t>
+  </si>
+  <si>
+    <t>10X2 header pins</t>
+  </si>
+  <si>
+    <t>1206 Capacitor</t>
+  </si>
+  <si>
+    <t>1206 Resistor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,13 +252,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -558,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -570,13 +608,13 @@
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -596,211 +634,230 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
       <c r="D6">
         <v>1206</v>
       </c>
       <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>1206</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1206</v>
       </c>
       <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>46</v>
       </c>
       <c r="G11" t="s">
         <v>47</v>
       </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>